<commit_message>
This version is only to store this version with UART already implemented but not validated
</commit_message>
<xml_diff>
--- a/CDI_code/Hardware/Hardware_Description_v1.xlsx
+++ b/CDI_code/Hardware/Hardware_Description_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A551633\Documents\My_Dev_Repo\V6_CDI\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A551633\Documents\My_Dev_Repo\Repo\CDI\CDI_code\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBFF28D-2EE1-463E-B88C-2A86669E03E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5FF745-45DA-4B60-8D41-6AF0D680104C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin_Description" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="201">
   <si>
     <t xml:space="preserve">Story </t>
   </si>
@@ -303,12 +303,6 @@
     <t>ADC12_IN1</t>
   </si>
   <si>
-    <t>VOLTMTR_PS</t>
-  </si>
-  <si>
-    <t>VOLTMTR_INV</t>
-  </si>
-  <si>
     <t>CDI_TRGGR</t>
   </si>
   <si>
@@ -316,9 +310,6 @@
   </si>
   <si>
     <t>CRKSHFT_SENS1</t>
-  </si>
-  <si>
-    <t>CRKSHFT_SENS2</t>
   </si>
   <si>
     <t>TIM1_CH1</t>
@@ -644,6 +635,30 @@
   <si>
     <t>TDuty</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Prepare to be available Serial connection in prototype board</t>
+  </si>
+  <si>
+    <t>I need to create the hardware connection to use the serial port (USART2), because I will leave USART1 free to use to upload new software in Bluepill</t>
+  </si>
+  <si>
+    <t>BLUEPILL_LED</t>
+  </si>
+  <si>
+    <t>RX from PC</t>
+  </si>
+  <si>
+    <t>TX from PC</t>
+  </si>
+  <si>
+    <t>USART3_TX</t>
+  </si>
+  <si>
+    <t>USART3_RX</t>
+  </si>
 </sst>
 </file>
 
@@ -815,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -944,6 +959,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8334,8 +8358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8356,13 +8380,13 @@
         <v>79</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -8393,7 +8417,9 @@
       <c r="D3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -8513,9 +8539,7 @@
       <c r="D11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -8530,9 +8554,7 @@
       <c r="D12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -8545,7 +8567,9 @@
         <v>6</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -8631,9 +8655,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -8646,9 +8668,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>165</v>
-      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -8675,8 +8695,12 @@
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -8688,8 +8712,12 @@
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -8784,11 +8812,9 @@
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>86</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -8923,7 +8949,9 @@
       <c r="D39" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -8983,7 +9011,9 @@
       <c r="D43" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -9026,11 +9056,9 @@
         <v>6</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -9085,7 +9113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230A22CC-38FC-438F-9D75-AAFE78B3F39C}">
   <dimension ref="A1:AR337"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6:F10"/>
     </sheetView>
   </sheetViews>
@@ -9105,34 +9133,34 @@
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M1" s="31"/>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
       <c r="P1" s="32"/>
       <c r="Q1" s="33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
       <c r="T1" s="34"/>
       <c r="U1" s="35"/>
       <c r="V1" s="36" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="W1" s="37"/>
       <c r="X1" s="37"/>
       <c r="Y1" s="37"/>
       <c r="Z1" s="38"/>
       <c r="AA1" s="39" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AB1" s="40"/>
       <c r="AC1" s="40"/>
@@ -9140,7 +9168,7 @@
       <c r="AE1" s="40"/>
       <c r="AF1" s="41"/>
       <c r="AG1" s="33" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AH1" s="34"/>
       <c r="AI1" s="34"/>
@@ -9148,7 +9176,7 @@
       <c r="AK1" s="34"/>
       <c r="AL1" s="35"/>
       <c r="AM1" s="42" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AN1" s="43"/>
       <c r="AO1" s="43"/>
@@ -9158,118 +9186,118 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1">
         <f>72000000/B1</f>
         <v>72000000</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N2" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA2" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB2" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF2" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH2" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q2" s="20" t="s">
+      <c r="AI2" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="R2" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="V2" s="18" t="s">
+      <c r="AJ2" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK2" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL2" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="AM2" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN2" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="W2" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z2" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA2" s="22" t="s">
+      <c r="AO2" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP2" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="AQ2" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="AR2" s="25" t="s">
         <v>166</v>
-      </c>
-      <c r="AB2" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC2" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD2" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="AE2" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG2" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH2" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI2" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="AJ2" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="AK2" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="AM2" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="AN2" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO2" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="AP2" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AQ2" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="AR2" s="25" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" s="1">
         <f>1/B2</f>
@@ -9409,27 +9437,27 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1">
         <v>55</v>
       </c>
       <c r="U4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>186</v>
+      </c>
+      <c r="AR4" t="s">
         <v>187</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>188</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>189</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -9437,7 +9465,7 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -9445,7 +9473,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1">
         <f>B5-B6</f>
@@ -9454,7 +9482,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1">
         <v>127</v>
@@ -9462,7 +9490,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B9" s="1">
         <f>B7/B8</f>
@@ -9471,7 +9499,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B10" s="1">
         <f>Sheet3!B65</f>
@@ -9481,7 +9509,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B11" s="1">
         <f>(B5-B10)/B9</f>
@@ -9490,7 +9518,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B12" s="1">
         <f>0.0015</f>
@@ -9499,7 +9527,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B13" s="2">
         <f>2^16*B3*B4</f>
@@ -9508,22 +9536,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="1"/>
@@ -13463,76 +13491,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="30.875" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
+    <col min="3" max="3" width="46.75" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="30.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="45">
+        <v>44223</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13564,19 +13610,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F1" s="6"/>
     </row>
@@ -13602,28 +13648,28 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -14700,18 +14746,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -14734,7 +14780,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B6" s="6">
         <f>65535*C21</f>
@@ -14793,7 +14839,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B15" s="6">
         <v>50</v>
@@ -14803,7 +14849,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B16" s="9">
         <v>15000</v>
@@ -14813,7 +14859,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B17" s="9">
         <v>15000</v>
@@ -14829,10 +14875,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C19" s="1">
         <v>72000000</v>
@@ -14842,10 +14888,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C20" s="1">
         <f>1/C19</f>
@@ -14856,10 +14902,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C21" s="6">
         <v>160</v>
@@ -14869,10 +14915,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C22" s="6">
         <v>40</v>
@@ -14882,10 +14928,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C23" s="6">
         <v>18</v>
@@ -14895,10 +14941,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C24" s="6">
         <v>0.2</v>
@@ -14908,10 +14954,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C25" s="6">
         <f>C22-C23</f>
@@ -14922,10 +14968,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C26" s="6">
         <f>C25/C24</f>
@@ -14936,10 +14982,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C27" s="6">
         <v>35</v>
@@ -14949,10 +14995,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C28" s="6">
         <f>C22-C27</f>
@@ -14963,10 +15009,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C29" s="6">
         <f>C28/C24</f>
@@ -14977,10 +15023,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C30" s="9">
         <v>5003</v>
@@ -14990,10 +15036,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C31" s="9">
         <f>C30/60</f>
@@ -15004,10 +15050,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C32" s="9">
         <f>1/C31</f>
@@ -15018,7 +15064,7 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C33" s="9">
         <f>C32/$C$20</f>
@@ -15029,7 +15075,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C34" s="9">
         <f>INT(C32/$C$20)</f>
@@ -15040,7 +15086,7 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C35" s="9">
         <f>C33-C34</f>
@@ -15051,7 +15097,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C36" s="9">
         <f>(C33-C34)/C33</f>
@@ -15062,7 +15108,7 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C37" s="9">
         <f>C33/$C$21</f>
@@ -15073,7 +15119,7 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C38" s="9">
         <f>INT(C34/$C$21)</f>
@@ -15084,7 +15130,7 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C39" s="9">
         <f>C37-C38</f>
@@ -15095,7 +15141,7 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C40" s="9">
         <f>INT(C39*$C$21)</f>
@@ -15106,7 +15152,7 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C41" s="9">
         <f>C38/(360/$C$24)</f>
@@ -15124,7 +15170,7 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C42" s="9">
         <f>INT(C38/(360/$C$24))</f>
@@ -15142,7 +15188,7 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C43" s="9">
         <f>ROUND(C38/(360/$C$24),0)</f>
@@ -15303,19 +15349,19 @@
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="D65" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -15387,7 +15433,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D69" s="1">
         <f t="shared" si="0"/>
@@ -15415,10 +15461,10 @@
         <v>50</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D70" s="1">
         <f t="shared" si="0"/>
@@ -16498,7 +16544,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -16507,7 +16553,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1">
         <f>72000000/B1</f>
@@ -16515,12 +16561,12 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" s="1">
         <f>1/B2</f>
@@ -16534,7 +16580,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -16547,7 +16593,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -16560,7 +16606,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -16573,7 +16619,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1">
         <f>B5-B6</f>
@@ -16586,7 +16632,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1">
         <v>128</v>
@@ -16598,7 +16644,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B9" s="1">
         <f>B7/B8</f>
@@ -16611,7 +16657,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B10" s="1">
         <f>Sheet3!B65</f>
@@ -16624,7 +16670,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B11" s="1">
         <f>(B5-B10)/B9</f>
@@ -16637,7 +16683,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B12" s="1">
         <f>0.0015</f>
@@ -16662,58 +16708,58 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="K15" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="P15" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -20312,7 +20358,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -20321,7 +20367,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1">
         <f>72000000/B1</f>
@@ -20329,12 +20375,12 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" s="1">
         <f>1/B2</f>
@@ -20348,7 +20394,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -20361,7 +20407,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -20374,7 +20420,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -20387,7 +20433,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1">
         <f>B5-B6</f>
@@ -20400,7 +20446,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1">
         <v>128</v>
@@ -20412,7 +20458,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B9" s="1">
         <f>B7/B8</f>
@@ -20425,7 +20471,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B10" s="1">
         <f>Sheet3!B65</f>
@@ -20438,7 +20484,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B11" s="1">
         <f>(B5-B10)/B9</f>
@@ -20451,7 +20497,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B12" s="1">
         <f>0.0015</f>
@@ -20476,58 +20522,58 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="K15" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="P15" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -22939,34 +22985,34 @@
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M1" s="31"/>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
       <c r="P1" s="32"/>
       <c r="Q1" s="33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="R1" s="34"/>
       <c r="S1" s="34"/>
       <c r="T1" s="34"/>
       <c r="U1" s="35"/>
       <c r="V1" s="36" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="W1" s="37"/>
       <c r="X1" s="37"/>
       <c r="Y1" s="37"/>
       <c r="Z1" s="38"/>
       <c r="AA1" s="39" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AB1" s="40"/>
       <c r="AC1" s="40"/>
@@ -22974,7 +23020,7 @@
       <c r="AE1" s="40"/>
       <c r="AF1" s="41"/>
       <c r="AG1" s="33" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AH1" s="34"/>
       <c r="AI1" s="34"/>
@@ -22982,7 +23028,7 @@
       <c r="AK1" s="34"/>
       <c r="AL1" s="35"/>
       <c r="AM1" s="42" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AN1" s="43"/>
       <c r="AO1" s="43"/>
@@ -22992,118 +23038,118 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1">
         <f>72000000/B1</f>
         <v>72000000</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N2" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA2" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB2" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF2" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH2" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q2" s="20" t="s">
+      <c r="AI2" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="R2" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="V2" s="18" t="s">
+      <c r="AJ2" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK2" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL2" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="AM2" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN2" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="W2" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z2" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA2" s="22" t="s">
+      <c r="AO2" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP2" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="AQ2" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="AR2" s="25" t="s">
         <v>166</v>
-      </c>
-      <c r="AB2" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC2" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD2" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="AE2" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG2" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH2" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI2" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="AJ2" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="AK2" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="AM2" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="AN2" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO2" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="AP2" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AQ2" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="AR2" s="25" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" s="1">
         <f>1/B2</f>
@@ -23243,27 +23289,27 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="U4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>186</v>
+      </c>
+      <c r="AR4" t="s">
         <v>187</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>188</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>189</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -23275,7 +23321,7 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -23286,7 +23332,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1">
         <f>B5-B6</f>
@@ -23299,7 +23345,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1">
         <v>127</v>
@@ -23311,7 +23357,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B9" s="1">
         <f>B7/B8</f>
@@ -23327,7 +23373,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B10" s="1">
         <f>Sheet3!B65</f>
@@ -23351,7 +23397,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B11" s="1">
         <f>(B5-B10)/B9</f>
@@ -23368,7 +23414,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B12" s="1">
         <f>0.0015</f>
@@ -23381,7 +23427,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B13" s="2">
         <f>2^16*B3</f>
@@ -23437,23 +23483,23 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H18" s="2"/>
       <c r="L18">
@@ -23497,7 +23543,7 @@
         <v>0</v>
       </c>
       <c r="V19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="W19">
         <f>R3+AA3</f>
@@ -23540,7 +23586,7 @@
         <v>1</v>
       </c>
       <c r="V20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="W20">
         <f>W19/B3</f>
@@ -23587,7 +23633,7 @@
         <v>2</v>
       </c>
       <c r="V21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="W21">
         <f>INT(W20/65536)</f>
@@ -23630,7 +23676,7 @@
         <v>3</v>
       </c>
       <c r="V22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="W22">
         <f>W20-(65536*W21)</f>

</xml_diff>

<commit_message>
Update new files during PCB development
</commit_message>
<xml_diff>
--- a/CDI_code/Hardware/Hardware_Description_v1.xlsx
+++ b/CDI_code/Hardware/Hardware_Description_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A551633\Documents\My_Dev_Repo\Repo\CDI\CDI_code\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Teste_Clone_CDI\CDI_do_Jerena\CDI_code\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5FF745-45DA-4B60-8D41-6AF0D680104C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F6097F-BE5E-43D8-9724-29B13C57B473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin_Description" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -303,13 +305,7 @@
     <t>ADC12_IN1</t>
   </si>
   <si>
-    <t>CDI_TRGGR</t>
-  </si>
-  <si>
     <t>MODULE</t>
-  </si>
-  <si>
-    <t>CRKSHFT_SENS1</t>
   </si>
   <si>
     <t>TIM1_CH1</t>
@@ -659,6 +655,12 @@
   <si>
     <t>USART3_RX</t>
   </si>
+  <si>
+    <t>VRS_SIGNAL</t>
+  </si>
+  <si>
+    <t>CDI_TRIGGER</t>
+  </si>
 </sst>
 </file>
 
@@ -915,6 +917,15 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -959,15 +970,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8359,17 +8361,17 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -8380,13 +8382,13 @@
         <v>79</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -8418,7 +8420,7 @@
         <v>55</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -8568,7 +8570,7 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -8696,10 +8698,10 @@
         <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -8713,10 +8715,10 @@
         <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -8812,7 +8814,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -8950,7 +8952,7 @@
         <v>69</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -9012,7 +9014,7 @@
         <v>75</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -9056,7 +9058,7 @@
         <v>6</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E46" s="1"/>
     </row>
@@ -9117,187 +9119,187 @@
       <selection activeCell="D6" sqref="D6:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="L1" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="33" t="s">
+      <c r="L1" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="41"/>
-      <c r="AG1" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="AN1" s="43"/>
-      <c r="AO1" s="43"/>
-      <c r="AP1" s="43"/>
-      <c r="AQ1" s="43"/>
-      <c r="AR1" s="44"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="47"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1">
         <f>72000000/B1</f>
         <v>72000000</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L2" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="Q2" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="T2" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA2" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB2" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF2" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG2" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="R2" s="20" t="s">
+      <c r="AH2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="AJ2" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="S2" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="V2" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="W2" s="19" t="s">
+      <c r="AK2" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL2" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM2" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="AN2" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="AO2" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP2" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="X2" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z2" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="AA2" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="AB2" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC2" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="AD2" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="AE2" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG2" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AH2" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="AI2" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="AJ2" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="AK2" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="AL2" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="AM2" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="AN2" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO2" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="AP2" s="25" t="s">
-        <v>175</v>
-      </c>
       <c r="AQ2" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AR2" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="1">
         <f>1/B2</f>
@@ -9437,27 +9439,27 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B4" s="1">
         <v>55</v>
       </c>
       <c r="U4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL4" t="s">
         <v>184</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AR4" t="s">
         <v>185</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>186</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -9465,7 +9467,7 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -9473,7 +9475,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1">
         <f>B5-B6</f>
@@ -9482,7 +9484,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B8" s="1">
         <v>127</v>
@@ -9490,7 +9492,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" s="1">
         <f>B7/B8</f>
@@ -9499,7 +9501,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B10" s="1">
         <f>Sheet3!B65</f>
@@ -9509,7 +9511,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" s="1">
         <f>(B5-B10)/B9</f>
@@ -9518,7 +9520,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1">
         <f>0.0015</f>
@@ -9527,7 +9529,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B13" s="2">
         <f>2^16*B3*B4</f>
@@ -9536,22 +9538,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="1"/>
@@ -13497,48 +13499,48 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.25" customWidth="1"/>
-    <col min="3" max="3" width="46.75" customWidth="1"/>
-    <col min="4" max="4" width="16.375" customWidth="1"/>
-    <col min="5" max="5" width="30.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" customWidth="1"/>
+    <col min="3" max="3" width="46.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="30.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="45">
+    <row r="2" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A2" s="30">
         <v>44223</v>
       </c>
-      <c r="B2" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="B2" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -13594,35 +13596,35 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="F1" s="6"/>
     </row>
@@ -13648,28 +13650,28 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -14730,34 +14732,34 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -14780,7 +14782,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6" s="6">
         <f>65535*C21</f>
@@ -14839,7 +14841,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B15" s="6">
         <v>50</v>
@@ -14849,7 +14851,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="9">
         <v>15000</v>
@@ -14859,7 +14861,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B17" s="9">
         <v>15000</v>
@@ -14875,10 +14877,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1">
         <v>72000000</v>
@@ -14888,10 +14890,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C20" s="1">
         <f>1/C19</f>
@@ -14902,10 +14904,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21" s="6">
         <v>160</v>
@@ -14915,10 +14917,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C22" s="6">
         <v>40</v>
@@ -14928,10 +14930,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C23" s="6">
         <v>18</v>
@@ -14941,10 +14943,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C24" s="6">
         <v>0.2</v>
@@ -14954,10 +14956,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C25" s="6">
         <f>C22-C23</f>
@@ -14968,10 +14970,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C26" s="6">
         <f>C25/C24</f>
@@ -14982,10 +14984,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C27" s="6">
         <v>35</v>
@@ -14995,10 +14997,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C28" s="6">
         <f>C22-C27</f>
@@ -15009,10 +15011,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29" s="6">
         <f>C28/C24</f>
@@ -15023,10 +15025,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C30" s="9">
         <v>5003</v>
@@ -15036,10 +15038,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C31" s="9">
         <f>C30/60</f>
@@ -15050,10 +15052,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="C32" s="9">
         <f>1/C31</f>
@@ -15064,7 +15066,7 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C33" s="9">
         <f>C32/$C$20</f>
@@ -15075,7 +15077,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C34" s="9">
         <f>INT(C32/$C$20)</f>
@@ -15086,7 +15088,7 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C35" s="9">
         <f>C33-C34</f>
@@ -15097,7 +15099,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C36" s="9">
         <f>(C33-C34)/C33</f>
@@ -15108,7 +15110,7 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C37" s="9">
         <f>C33/$C$21</f>
@@ -15119,7 +15121,7 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C38" s="9">
         <f>INT(C34/$C$21)</f>
@@ -15130,7 +15132,7 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C39" s="9">
         <f>C37-C38</f>
@@ -15141,7 +15143,7 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C40" s="9">
         <f>INT(C39*$C$21)</f>
@@ -15152,7 +15154,7 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C41" s="9">
         <f>C38/(360/$C$24)</f>
@@ -15170,7 +15172,7 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C42" s="9">
         <f>INT(C38/(360/$C$24))</f>
@@ -15188,7 +15190,7 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C43" s="9">
         <f>ROUND(C38/(360/$C$24),0)</f>
@@ -15349,19 +15351,19 @@
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="D65" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -15433,7 +15435,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D69" s="1">
         <f t="shared" si="0"/>
@@ -15461,10 +15463,10 @@
         <v>50</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D70" s="1">
         <f t="shared" si="0"/>
@@ -16443,7 +16445,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -16519,32 +16521,32 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -16553,7 +16555,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1">
         <f>72000000/B1</f>
@@ -16561,12 +16563,12 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="1">
         <f>1/B2</f>
@@ -16580,7 +16582,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -16593,7 +16595,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -16606,7 +16608,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -16619,7 +16621,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1">
         <f>B5-B6</f>
@@ -16632,7 +16634,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B8" s="1">
         <v>128</v>
@@ -16644,7 +16646,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" s="1">
         <f>B7/B8</f>
@@ -16657,7 +16659,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B10" s="1">
         <f>Sheet3!B65</f>
@@ -16670,7 +16672,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" s="1">
         <f>(B5-B10)/B9</f>
@@ -16683,7 +16685,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1">
         <f>0.0015</f>
@@ -16708,58 +16710,58 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P15" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -19156,7 +19158,7 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
@@ -20333,32 +20335,32 @@
       <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -20367,7 +20369,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1">
         <f>72000000/B1</f>
@@ -20375,12 +20377,12 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="1">
         <f>1/B2</f>
@@ -20394,7 +20396,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -20407,7 +20409,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -20420,7 +20422,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -20433,7 +20435,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1">
         <f>B5-B6</f>
@@ -20446,7 +20448,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B8" s="1">
         <v>128</v>
@@ -20458,7 +20460,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" s="1">
         <f>B7/B8</f>
@@ -20471,7 +20473,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B10" s="1">
         <f>Sheet3!B65</f>
@@ -20484,7 +20486,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" s="1">
         <f>(B5-B10)/B9</f>
@@ -20497,7 +20499,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1">
         <f>0.0015</f>
@@ -20522,58 +20524,58 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P15" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -22970,186 +22972,186 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="L1" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="33" t="s">
+      <c r="L1" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="41"/>
-      <c r="AG1" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="AN1" s="43"/>
-      <c r="AO1" s="43"/>
-      <c r="AP1" s="43"/>
-      <c r="AQ1" s="43"/>
-      <c r="AR1" s="44"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="47"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1">
         <f>72000000/B1</f>
         <v>72000000</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L2" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="Q2" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="T2" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA2" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB2" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF2" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG2" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="R2" s="20" t="s">
+      <c r="AH2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="AJ2" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="S2" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="V2" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="W2" s="19" t="s">
+      <c r="AK2" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL2" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM2" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="AN2" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="AO2" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP2" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="X2" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z2" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="AA2" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="AB2" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC2" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="AD2" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="AE2" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG2" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AH2" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="AI2" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="AJ2" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="AK2" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="AL2" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="AM2" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="AN2" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO2" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="AP2" s="25" t="s">
-        <v>175</v>
-      </c>
       <c r="AQ2" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AR2" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="1">
         <f>1/B2</f>
@@ -23289,27 +23291,27 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="U4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL4" t="s">
         <v>184</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AR4" t="s">
         <v>185</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>186</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -23321,7 +23323,7 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -23332,7 +23334,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1">
         <f>B5-B6</f>
@@ -23345,7 +23347,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B8" s="1">
         <v>127</v>
@@ -23357,7 +23359,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" s="1">
         <f>B7/B8</f>
@@ -23373,7 +23375,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B10" s="1">
         <f>Sheet3!B65</f>
@@ -23397,7 +23399,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" s="1">
         <f>(B5-B10)/B9</f>
@@ -23414,7 +23416,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1">
         <f>0.0015</f>
@@ -23427,7 +23429,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B13" s="2">
         <f>2^16*B3</f>
@@ -23483,23 +23485,23 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H18" s="2"/>
       <c r="L18">
@@ -23543,7 +23545,7 @@
         <v>0</v>
       </c>
       <c r="V19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="W19">
         <f>R3+AA3</f>
@@ -23586,7 +23588,7 @@
         <v>1</v>
       </c>
       <c r="V20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="W20">
         <f>W19/B3</f>
@@ -23633,7 +23635,7 @@
         <v>2</v>
       </c>
       <c r="V21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="W21">
         <f>INT(W20/65536)</f>
@@ -23676,7 +23678,7 @@
         <v>3</v>
       </c>
       <c r="V22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="W22">
         <f>W20-(65536*W21)</f>

</xml_diff>

<commit_message>
More files was included and I update Hardware description
</commit_message>
<xml_diff>
--- a/CDI_code/Hardware/Hardware_Description_v1.xlsx
+++ b/CDI_code/Hardware/Hardware_Description_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Teste_Clone_CDI\CDI_do_Jerena\CDI_code\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A551633\Documents\My_Dev_Repo\Repo\CDI\CDI_code\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F6097F-BE5E-43D8-9724-29B13C57B473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E945D70-E2DC-4036-B753-7D713E4E6927}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin_Description" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="205">
   <si>
     <t xml:space="preserve">Story </t>
   </si>
@@ -661,6 +659,18 @@
   <si>
     <t>CDI_TRIGGER</t>
   </si>
+  <si>
+    <t>BOOTLOADER</t>
+  </si>
+  <si>
+    <t>Boot0 = 1, Boot1=0</t>
+  </si>
+  <si>
+    <t>Need to use the software Flash Loader ST (detailed information in AN2606) https://www.electronicshub.org/how-to-upload-stm32f103c8t6-usb-bootloader/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=K2NekHIwGWo</t>
+  </si>
 </sst>
 </file>
 
@@ -724,7 +734,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -828,11 +838,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -970,6 +991,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8358,20 +8382,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -8616,7 +8640,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -8631,7 +8655,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -8646,7 +8670,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -8659,7 +8683,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -8672,7 +8696,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -8687,7 +8711,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -8704,7 +8728,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -8721,7 +8745,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -8736,7 +8760,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -8751,7 +8775,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -8764,7 +8788,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -8777,7 +8801,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -8790,7 +8814,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -8803,7 +8827,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -8818,7 +8842,7 @@
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -8831,9 +8855,14 @@
       <c r="D31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F31" s="48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -8846,7 +8875,15 @@
       <c r="D32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>202</v>
+      </c>
+      <c r="H32" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -9119,16 +9156,16 @@
       <selection activeCell="D6" sqref="D6:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -13499,13 +13536,13 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
-    <col min="3" max="3" width="46.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" customWidth="1"/>
-    <col min="5" max="5" width="30.90625" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
+    <col min="3" max="3" width="46.75" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="30.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -13528,7 +13565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="30">
         <v>44223</v>
       </c>
@@ -13596,16 +13633,16 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -14732,16 +14769,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -16445,7 +16482,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -16521,26 +16558,26 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19158,7 +19195,7 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
@@ -20335,26 +20372,26 @@
       <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22972,15 +23009,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>